<commit_message>
update net premium reserves
</commit_message>
<xml_diff>
--- a/exercisesLifeContingencies/netPremiumReserves/wli_55_1_netReserves.xlsx
+++ b/exercisesLifeContingencies/netPremiumReserves/wli_55_1_netReserves.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E217"/>
+  <dimension ref="A1:E220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1834,20 +1834,20 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>GRF95</t>
+          <t>TV7377</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="C74" t="n">
-        <v>268.4632394670858</v>
+        <v>961.5384615384614</v>
       </c>
       <c r="D74" t="n">
-        <v>268.4632394670858</v>
+        <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>-5.684341886080801e-14</v>
+        <v>961.5384615384614</v>
       </c>
     </row>
     <row r="75">
@@ -1857,16 +1857,16 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C75" t="n">
-        <v>277.5114347986241</v>
+        <v>268.4632394670858</v>
       </c>
       <c r="D75" t="n">
-        <v>246.2851168918114</v>
+        <v>268.4632394670858</v>
       </c>
       <c r="E75" t="n">
-        <v>31.22631790681262</v>
+        <v>-5.684341886080801e-14</v>
       </c>
     </row>
     <row r="76">
@@ -1876,16 +1876,16 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C76" t="n">
-        <v>286.8279636588654</v>
+        <v>277.5114347986241</v>
       </c>
       <c r="D76" t="n">
-        <v>223.2019781822713</v>
+        <v>246.2851168918114</v>
       </c>
       <c r="E76" t="n">
-        <v>63.62598547659411</v>
+        <v>31.22631790681262</v>
       </c>
     </row>
     <row r="77">
@@ -1895,16 +1895,16 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C77" t="n">
-        <v>296.414699656469</v>
+        <v>286.8279636588654</v>
       </c>
       <c r="D77" t="n">
-        <v>199.171194385391</v>
+        <v>223.2019781822713</v>
       </c>
       <c r="E77" t="n">
-        <v>97.24350527107799</v>
+        <v>63.62598547659411</v>
       </c>
     </row>
     <row r="78">
@@ -1914,16 +1914,16 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C78" t="n">
-        <v>306.2730070395051</v>
+        <v>296.414699656469</v>
       </c>
       <c r="D78" t="n">
-        <v>174.1468112371373</v>
+        <v>199.171194385391</v>
       </c>
       <c r="E78" t="n">
-        <v>132.1261958023678</v>
+        <v>97.24350527107799</v>
       </c>
     </row>
     <row r="79">
@@ -1933,16 +1933,16 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C79" t="n">
-        <v>316.4039592796032</v>
+        <v>306.2730070395051</v>
       </c>
       <c r="D79" t="n">
-        <v>148.0790456094288</v>
+        <v>174.1468112371373</v>
       </c>
       <c r="E79" t="n">
-        <v>168.3249136701744</v>
+        <v>132.1261958023678</v>
       </c>
     </row>
     <row r="80">
@@ -1952,16 +1952,16 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C80" t="n">
-        <v>326.8084264756632</v>
+        <v>316.4039592796032</v>
       </c>
       <c r="D80" t="n">
-        <v>120.9137790284626</v>
+        <v>148.0790456094288</v>
       </c>
       <c r="E80" t="n">
-        <v>205.8946474472005</v>
+        <v>168.3249136701744</v>
       </c>
     </row>
     <row r="81">
@@ -1971,16 +1971,16 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C81" t="n">
-        <v>337.5014663007623</v>
+        <v>326.8084264756632</v>
       </c>
       <c r="D81" t="n">
-        <v>92.58999709171864</v>
+        <v>120.9137790284626</v>
       </c>
       <c r="E81" t="n">
-        <v>244.9114692090436</v>
+        <v>205.8946474472005</v>
       </c>
     </row>
     <row r="82">
@@ -1990,16 +1990,16 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C82" t="n">
-        <v>348.4986522250456</v>
+        <v>337.5014663007623</v>
       </c>
       <c r="D82" t="n">
-        <v>63.04292817913528</v>
+        <v>92.58999709171864</v>
       </c>
       <c r="E82" t="n">
-        <v>285.4557240459104</v>
+        <v>244.9114692090436</v>
       </c>
     </row>
     <row r="83">
@@ -2009,16 +2009,16 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C83" t="n">
-        <v>359.7968640940451</v>
+        <v>348.4986522250456</v>
       </c>
       <c r="D83" t="n">
-        <v>32.20467385907486</v>
+        <v>63.04292817913528</v>
       </c>
       <c r="E83" t="n">
-        <v>327.5921902349703</v>
+        <v>285.4557240459104</v>
       </c>
     </row>
     <row r="84">
@@ -2028,16 +2028,16 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C84" t="n">
-        <v>371.3765918414097</v>
+        <v>359.7968640940451</v>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>32.20467385907486</v>
       </c>
       <c r="E84" t="n">
-        <v>371.3765918414097</v>
+        <v>327.5921902349703</v>
       </c>
     </row>
     <row r="85">
@@ -2047,16 +2047,16 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C85" t="n">
-        <v>383.2040509194089</v>
+        <v>371.3765918414097</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
       </c>
       <c r="E85" t="n">
-        <v>383.2040509194089</v>
+        <v>371.3765918414097</v>
       </c>
     </row>
     <row r="86">
@@ -2066,16 +2066,16 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C86" t="n">
-        <v>395.2372234443999</v>
+        <v>383.2040509194089</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>395.2372234443999</v>
+        <v>383.2040509194089</v>
       </c>
     </row>
     <row r="87">
@@ -2085,16 +2085,16 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C87" t="n">
-        <v>407.4423620377428</v>
+        <v>395.2372234443999</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>407.4423620377428</v>
+        <v>395.2372234443999</v>
       </c>
     </row>
     <row r="88">
@@ -2104,16 +2104,16 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C88" t="n">
-        <v>419.7973474138689</v>
+        <v>407.4423620377428</v>
       </c>
       <c r="D88" t="n">
         <v>0</v>
       </c>
       <c r="E88" t="n">
-        <v>419.7973474138689</v>
+        <v>407.4423620377428</v>
       </c>
     </row>
     <row r="89">
@@ -2123,16 +2123,16 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C89" t="n">
-        <v>432.2906025236726</v>
+        <v>419.7973474138689</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>432.2906025236726</v>
+        <v>419.7973474138689</v>
       </c>
     </row>
     <row r="90">
@@ -2142,16 +2142,16 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C90" t="n">
-        <v>444.9204465025264</v>
+        <v>432.2906025236726</v>
       </c>
       <c r="D90" t="n">
         <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>444.9204465025264</v>
+        <v>432.2906025236726</v>
       </c>
     </row>
     <row r="91">
@@ -2161,16 +2161,16 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C91" t="n">
-        <v>457.694484912438</v>
+        <v>444.9204465025264</v>
       </c>
       <c r="D91" t="n">
         <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>457.694484912438</v>
+        <v>444.9204465025264</v>
       </c>
     </row>
     <row r="92">
@@ -2180,16 +2180,16 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C92" t="n">
-        <v>470.6287758236891</v>
+        <v>457.694484912438</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
       </c>
       <c r="E92" t="n">
-        <v>470.6287758236891</v>
+        <v>457.694484912438</v>
       </c>
     </row>
     <row r="93">
@@ -2199,16 +2199,16 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C93" t="n">
-        <v>483.7473735746562</v>
+        <v>470.6287758236891</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>483.7473735746562</v>
+        <v>470.6287758236891</v>
       </c>
     </row>
     <row r="94">
@@ -2218,16 +2218,16 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C94" t="n">
-        <v>497.0818647013352</v>
+        <v>483.7473735746562</v>
       </c>
       <c r="D94" t="n">
         <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>497.0818647013352</v>
+        <v>483.7473735746562</v>
       </c>
     </row>
     <row r="95">
@@ -2237,16 +2237,16 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C95" t="n">
-        <v>510.6635625147411</v>
+        <v>497.0818647013352</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>510.6635625147411</v>
+        <v>497.0818647013352</v>
       </c>
     </row>
     <row r="96">
@@ -2256,16 +2256,16 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C96" t="n">
-        <v>524.4957647301854</v>
+        <v>510.6635625147411</v>
       </c>
       <c r="D96" t="n">
         <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>524.4957647301854</v>
+        <v>510.6635625147411</v>
       </c>
     </row>
     <row r="97">
@@ -2275,16 +2275,16 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C97" t="n">
-        <v>538.5519831294657</v>
+        <v>524.4957647301854</v>
       </c>
       <c r="D97" t="n">
         <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>538.5519831294657</v>
+        <v>524.4957647301854</v>
       </c>
     </row>
     <row r="98">
@@ -2294,16 +2294,16 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C98" t="n">
-        <v>552.7811396502045</v>
+        <v>538.5519831294657</v>
       </c>
       <c r="D98" t="n">
         <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>552.7811396502045</v>
+        <v>538.5519831294657</v>
       </c>
     </row>
     <row r="99">
@@ -2313,16 +2313,16 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C99" t="n">
-        <v>567.1127079789268</v>
+        <v>552.7811396502045</v>
       </c>
       <c r="D99" t="n">
         <v>0</v>
       </c>
       <c r="E99" t="n">
-        <v>567.1127079789268</v>
+        <v>552.7811396502045</v>
       </c>
     </row>
     <row r="100">
@@ -2332,16 +2332,16 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C100" t="n">
-        <v>581.4611358876722</v>
+        <v>567.1127079789268</v>
       </c>
       <c r="D100" t="n">
         <v>0</v>
       </c>
       <c r="E100" t="n">
-        <v>581.4611358876722</v>
+        <v>567.1127079789268</v>
       </c>
     </row>
     <row r="101">
@@ -2351,16 +2351,16 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C101" t="n">
-        <v>595.7297427588564</v>
+        <v>581.4611358876722</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>595.7297427588564</v>
+        <v>581.4611358876722</v>
       </c>
     </row>
     <row r="102">
@@ -2370,16 +2370,16 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C102" t="n">
-        <v>609.8138379796719</v>
+        <v>595.7297427588564</v>
       </c>
       <c r="D102" t="n">
         <v>0</v>
       </c>
       <c r="E102" t="n">
-        <v>609.8138379796719</v>
+        <v>595.7297427588564</v>
       </c>
     </row>
     <row r="103">
@@ -2389,16 +2389,16 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C103" t="n">
-        <v>623.6101515688712</v>
+        <v>609.8138379796719</v>
       </c>
       <c r="D103" t="n">
         <v>0</v>
       </c>
       <c r="E103" t="n">
-        <v>623.6101515688712</v>
+        <v>609.8138379796719</v>
       </c>
     </row>
     <row r="104">
@@ -2408,16 +2408,16 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C104" t="n">
-        <v>637.043988455098</v>
+        <v>623.6101515688712</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>637.043988455098</v>
+        <v>623.6101515688712</v>
       </c>
     </row>
     <row r="105">
@@ -2427,16 +2427,16 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C105" t="n">
-        <v>650.071622058163</v>
+        <v>637.043988455098</v>
       </c>
       <c r="D105" t="n">
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>650.071622058163</v>
+        <v>637.043988455098</v>
       </c>
     </row>
     <row r="106">
@@ -2446,16 +2446,16 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C106" t="n">
-        <v>662.6761172470974</v>
+        <v>650.071622058163</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
       </c>
       <c r="E106" t="n">
-        <v>662.6761172470974</v>
+        <v>650.071622058163</v>
       </c>
     </row>
     <row r="107">
@@ -2465,16 +2465,16 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C107" t="n">
-        <v>674.8636702712317</v>
+        <v>662.6761172470974</v>
       </c>
       <c r="D107" t="n">
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>674.8636702712317</v>
+        <v>662.6761172470974</v>
       </c>
     </row>
     <row r="108">
@@ -2484,16 +2484,16 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C108" t="n">
-        <v>686.6609273873895</v>
+        <v>674.8636702712317</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
       </c>
       <c r="E108" t="n">
-        <v>686.6609273873895</v>
+        <v>674.8636702712317</v>
       </c>
     </row>
     <row r="109">
@@ -2503,16 +2503,16 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C109" t="n">
-        <v>698.1130465061137</v>
+        <v>686.6609273873895</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>698.1130465061137</v>
+        <v>686.6609273873895</v>
       </c>
     </row>
     <row r="110">
@@ -2522,16 +2522,16 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C110" t="n">
-        <v>709.2826556600119</v>
+        <v>698.1130465061137</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
       </c>
       <c r="E110" t="n">
-        <v>709.2826556600119</v>
+        <v>698.1130465061137</v>
       </c>
     </row>
     <row r="111">
@@ -2541,16 +2541,16 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C111" t="n">
-        <v>720.2494492199627</v>
+        <v>709.2826556600119</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>720.2494492199627</v>
+        <v>709.2826556600119</v>
       </c>
     </row>
     <row r="112">
@@ -2560,16 +2560,16 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C112" t="n">
-        <v>731.0952738486961</v>
+        <v>720.2494492199627</v>
       </c>
       <c r="D112" t="n">
         <v>0</v>
       </c>
       <c r="E112" t="n">
-        <v>731.0952738486961</v>
+        <v>720.2494492199627</v>
       </c>
     </row>
     <row r="113">
@@ -2579,16 +2579,16 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C113" t="n">
-        <v>741.848715051817</v>
+        <v>731.0952738486961</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
       </c>
       <c r="E113" t="n">
-        <v>741.848715051817</v>
+        <v>731.0952738486961</v>
       </c>
     </row>
     <row r="114">
@@ -2598,16 +2598,16 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C114" t="n">
-        <v>752.4806001959223</v>
+        <v>741.848715051817</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>752.4806001959223</v>
+        <v>741.848715051817</v>
       </c>
     </row>
     <row r="115">
@@ -2617,16 +2617,16 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C115" t="n">
-        <v>762.9128784631893</v>
+        <v>752.4806001959223</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>762.9128784631893</v>
+        <v>752.4806001959223</v>
       </c>
     </row>
     <row r="116">
@@ -2636,16 +2636,16 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C116" t="n">
-        <v>773.0752162784649</v>
+        <v>762.9128784631893</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
       </c>
       <c r="E116" t="n">
-        <v>773.0752162784649</v>
+        <v>762.9128784631893</v>
       </c>
     </row>
     <row r="117">
@@ -2655,16 +2655,16 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C117" t="n">
-        <v>782.9376890953911</v>
+        <v>773.0752162784649</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>782.9376890953911</v>
+        <v>773.0752162784649</v>
       </c>
     </row>
     <row r="118">
@@ -2674,16 +2674,16 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C118" t="n">
-        <v>792.4775407595641</v>
+        <v>782.9376890953911</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>792.4775407595641</v>
+        <v>782.9376890953911</v>
       </c>
     </row>
     <row r="119">
@@ -2693,16 +2693,16 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C119" t="n">
-        <v>801.6783390454493</v>
+        <v>792.4775407595641</v>
       </c>
       <c r="D119" t="n">
         <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>801.6783390454493</v>
+        <v>792.4775407595641</v>
       </c>
     </row>
     <row r="120">
@@ -2712,16 +2712,16 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C120" t="n">
-        <v>810.5291984586411</v>
+        <v>801.6783390454493</v>
       </c>
       <c r="D120" t="n">
         <v>0</v>
       </c>
       <c r="E120" t="n">
-        <v>810.5291984586411</v>
+        <v>801.6783390454493</v>
       </c>
     </row>
     <row r="121">
@@ -2731,16 +2731,16 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C121" t="n">
-        <v>819.0240625349516</v>
+        <v>810.5291984586411</v>
       </c>
       <c r="D121" t="n">
         <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>819.0240625349516</v>
+        <v>810.5291984586411</v>
       </c>
     </row>
     <row r="122">
@@ -2750,16 +2750,16 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C122" t="n">
-        <v>827.1609174942937</v>
+        <v>819.0240625349516</v>
       </c>
       <c r="D122" t="n">
         <v>0</v>
       </c>
       <c r="E122" t="n">
-        <v>827.1609174942937</v>
+        <v>819.0240625349516</v>
       </c>
     </row>
     <row r="123">
@@ -2769,16 +2769,16 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C123" t="n">
-        <v>834.9411990708055</v>
+        <v>827.1609174942937</v>
       </c>
       <c r="D123" t="n">
         <v>0</v>
       </c>
       <c r="E123" t="n">
-        <v>834.9411990708055</v>
+        <v>827.1609174942937</v>
       </c>
     </row>
     <row r="124">
@@ -2788,16 +2788,16 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C124" t="n">
-        <v>842.3691673554475</v>
+        <v>834.9411990708055</v>
       </c>
       <c r="D124" t="n">
         <v>0</v>
       </c>
       <c r="E124" t="n">
-        <v>842.3691673554475</v>
+        <v>834.9411990708055</v>
       </c>
     </row>
     <row r="125">
@@ -2807,16 +2807,16 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C125" t="n">
-        <v>849.4514156251474</v>
+        <v>842.3691673554475</v>
       </c>
       <c r="D125" t="n">
         <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>849.4514156251474</v>
+        <v>842.3691673554475</v>
       </c>
     </row>
     <row r="126">
@@ -2826,16 +2826,16 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C126" t="n">
-        <v>856.1963904682134</v>
+        <v>849.4514156251474</v>
       </c>
       <c r="D126" t="n">
         <v>0</v>
       </c>
       <c r="E126" t="n">
-        <v>856.1963904682134</v>
+        <v>849.4514156251474</v>
       </c>
     </row>
     <row r="127">
@@ -2845,16 +2845,16 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C127" t="n">
-        <v>862.6139721675191</v>
+        <v>856.1963904682134</v>
       </c>
       <c r="D127" t="n">
         <v>0</v>
       </c>
       <c r="E127" t="n">
-        <v>862.6139721675191</v>
+        <v>856.1963904682134</v>
       </c>
     </row>
     <row r="128">
@@ -2864,16 +2864,16 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C128" t="n">
-        <v>868.7151612098397</v>
+        <v>862.6139721675191</v>
       </c>
       <c r="D128" t="n">
         <v>0</v>
       </c>
       <c r="E128" t="n">
-        <v>868.7151612098397</v>
+        <v>862.6139721675191</v>
       </c>
     </row>
     <row r="129">
@@ -2883,16 +2883,16 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C129" t="n">
-        <v>874.5117775023273</v>
+        <v>868.7151612098397</v>
       </c>
       <c r="D129" t="n">
         <v>0</v>
       </c>
       <c r="E129" t="n">
-        <v>874.5117775023273</v>
+        <v>868.7151612098397</v>
       </c>
     </row>
     <row r="130">
@@ -2902,16 +2902,16 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C130" t="n">
-        <v>880.0162164444313</v>
+        <v>874.5117775023273</v>
       </c>
       <c r="D130" t="n">
         <v>0</v>
       </c>
       <c r="E130" t="n">
-        <v>880.0162164444313</v>
+        <v>874.5117775023273</v>
       </c>
     </row>
     <row r="131">
@@ -2921,16 +2921,16 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C131" t="n">
-        <v>885.2413100066182</v>
+        <v>880.0162164444313</v>
       </c>
       <c r="D131" t="n">
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>885.2413100066182</v>
+        <v>880.0162164444313</v>
       </c>
     </row>
     <row r="132">
@@ -2940,16 +2940,16 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C132" t="n">
-        <v>890.2002232648599</v>
+        <v>885.2413100066182</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>890.2002232648599</v>
+        <v>885.2413100066182</v>
       </c>
     </row>
     <row r="133">
@@ -2959,16 +2959,16 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C133" t="n">
-        <v>894.9064516827735</v>
+        <v>890.2002232648599</v>
       </c>
       <c r="D133" t="n">
         <v>0</v>
       </c>
       <c r="E133" t="n">
-        <v>894.9064516827735</v>
+        <v>890.2002232648599</v>
       </c>
     </row>
     <row r="134">
@@ -2978,16 +2978,16 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C134" t="n">
-        <v>899.3740176604549</v>
+        <v>894.9064516827735</v>
       </c>
       <c r="D134" t="n">
         <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>899.3740176604549</v>
+        <v>894.9064516827735</v>
       </c>
     </row>
     <row r="135">
@@ -2997,16 +2997,16 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C135" t="n">
-        <v>903.6178993370435</v>
+        <v>899.3740176604549</v>
       </c>
       <c r="D135" t="n">
         <v>0</v>
       </c>
       <c r="E135" t="n">
-        <v>903.6178993370435</v>
+        <v>899.3740176604549</v>
       </c>
     </row>
     <row r="136">
@@ -3016,16 +3016,16 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C136" t="n">
-        <v>907.6550529021633</v>
+        <v>903.6178993370435</v>
       </c>
       <c r="D136" t="n">
         <v>0</v>
       </c>
       <c r="E136" t="n">
-        <v>907.6550529021633</v>
+        <v>903.6178993370435</v>
       </c>
     </row>
     <row r="137">
@@ -3035,16 +3035,16 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C137" t="n">
-        <v>911.5064066410372</v>
+        <v>907.6550529021633</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
       </c>
       <c r="E137" t="n">
-        <v>911.5064066410372</v>
+        <v>907.6550529021633</v>
       </c>
     </row>
     <row r="138">
@@ -3054,16 +3054,16 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C138" t="n">
-        <v>915.2012060223954</v>
+        <v>911.5064066410372</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
       </c>
       <c r="E138" t="n">
-        <v>915.2012060223954</v>
+        <v>911.5064066410372</v>
       </c>
     </row>
     <row r="139">
@@ -3073,16 +3073,16 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C139" t="n">
-        <v>918.7860843790783</v>
+        <v>915.2012060223954</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
       </c>
       <c r="E139" t="n">
-        <v>918.7860843790783</v>
+        <v>915.2012060223954</v>
       </c>
     </row>
     <row r="140">
@@ -3092,16 +3092,16 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C140" t="n">
-        <v>922.3451232955723</v>
+        <v>918.7860843790783</v>
       </c>
       <c r="D140" t="n">
         <v>0</v>
       </c>
       <c r="E140" t="n">
-        <v>922.3451232955723</v>
+        <v>918.7860843790783</v>
       </c>
     </row>
     <row r="141">
@@ -3111,16 +3111,16 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C141" t="n">
-        <v>926.0453945733609</v>
+        <v>922.3451232955723</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
       </c>
       <c r="E141" t="n">
-        <v>926.0453945733609</v>
+        <v>922.3451232955723</v>
       </c>
     </row>
     <row r="142">
@@ -3130,16 +3130,16 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C142" t="n">
-        <v>930.244698367111</v>
+        <v>926.0453945733609</v>
       </c>
       <c r="D142" t="n">
         <v>0</v>
       </c>
       <c r="E142" t="n">
-        <v>930.244698367111</v>
+        <v>926.0453945733609</v>
       </c>
     </row>
     <row r="143">
@@ -3149,16 +3149,16 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C143" t="n">
-        <v>935.7571199545279</v>
+        <v>930.244698367111</v>
       </c>
       <c r="D143" t="n">
         <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>935.7571199545279</v>
+        <v>930.244698367111</v>
       </c>
     </row>
     <row r="144">
@@ -3168,16 +3168,16 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C144" t="n">
-        <v>944.5379622781065</v>
+        <v>935.7571199545279</v>
       </c>
       <c r="D144" t="n">
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>944.5379622781065</v>
+        <v>935.7571199545279</v>
       </c>
     </row>
     <row r="145">
@@ -3187,54 +3187,54 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C145" t="n">
-        <v>961.5384615384615</v>
+        <v>944.5379622781065</v>
       </c>
       <c r="D145" t="n">
         <v>0</v>
       </c>
       <c r="E145" t="n">
-        <v>961.5384615384615</v>
+        <v>944.5379622781065</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>GRM95</t>
+          <t>GRF95</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>55</v>
+        <v>126</v>
       </c>
       <c r="C146" t="n">
-        <v>364.1816620555787</v>
+        <v>961.5384615384615</v>
       </c>
       <c r="D146" t="n">
-        <v>364.1816620555787</v>
+        <v>0</v>
       </c>
       <c r="E146" t="n">
-        <v>0</v>
+        <v>961.5384615384615</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>GRM95</t>
+          <t>GRF95</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="C147" t="n">
-        <v>374.8286037461733</v>
+        <v>961.5384615384614</v>
       </c>
       <c r="D147" t="n">
-        <v>334.4617697728315</v>
+        <v>0</v>
       </c>
       <c r="E147" t="n">
-        <v>40.36683397334178</v>
+        <v>961.5384615384614</v>
       </c>
     </row>
     <row r="148">
@@ -3244,16 +3244,16 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C148" t="n">
-        <v>385.65334440313</v>
+        <v>364.1816620555787</v>
       </c>
       <c r="D148" t="n">
-        <v>303.5151193693159</v>
+        <v>364.1816620555787</v>
       </c>
       <c r="E148" t="n">
-        <v>82.13822503381414</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -3263,16 +3263,16 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C149" t="n">
-        <v>396.6466410510574</v>
+        <v>374.8286037461733</v>
       </c>
       <c r="D149" t="n">
-        <v>271.2642005949982</v>
+        <v>334.4617697728315</v>
       </c>
       <c r="E149" t="n">
-        <v>125.3824404560592</v>
+        <v>40.36683397334178</v>
       </c>
     </row>
     <row r="150">
@@ -3282,16 +3282,16 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C150" t="n">
-        <v>407.7973298128023</v>
+        <v>385.65334440313</v>
       </c>
       <c r="D150" t="n">
-        <v>237.6222390172153</v>
+        <v>303.5151193693159</v>
       </c>
       <c r="E150" t="n">
-        <v>170.175090795587</v>
+        <v>82.13822503381414</v>
       </c>
     </row>
     <row r="151">
@@ -3301,16 +3301,16 @@
         </is>
       </c>
       <c r="B151" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C151" t="n">
-        <v>419.0924472893499</v>
+        <v>396.6466410510574</v>
       </c>
       <c r="D151" t="n">
-        <v>202.4913626036234</v>
+        <v>271.2642005949982</v>
       </c>
       <c r="E151" t="n">
-        <v>216.6010846857266</v>
+        <v>125.3824404560592</v>
       </c>
     </row>
     <row r="152">
@@ -3320,16 +3320,16 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C152" t="n">
-        <v>430.5175892697745</v>
+        <v>407.7973298128023</v>
       </c>
       <c r="D152" t="n">
-        <v>165.7604199577587</v>
+        <v>237.6222390172153</v>
       </c>
       <c r="E152" t="n">
-        <v>264.7571693120158</v>
+        <v>170.175090795587</v>
       </c>
     </row>
     <row r="153">
@@ -3339,16 +3339,16 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C153" t="n">
-        <v>442.0568695316322</v>
+        <v>419.0924472893499</v>
       </c>
       <c r="D153" t="n">
-        <v>127.3026323701055</v>
+        <v>202.4913626036234</v>
       </c>
       <c r="E153" t="n">
-        <v>314.7542371615267</v>
+        <v>216.6010846857266</v>
       </c>
     </row>
     <row r="154">
@@ -3358,16 +3358,16 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C154" t="n">
-        <v>453.6932770715935</v>
+        <v>430.5175892697745</v>
       </c>
       <c r="D154" t="n">
-        <v>86.97274601969887</v>
+        <v>165.7604199577587</v>
       </c>
       <c r="E154" t="n">
-        <v>366.7205310518946</v>
+        <v>264.7571693120158</v>
       </c>
     </row>
     <row r="155">
@@ -3377,16 +3377,16 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C155" t="n">
-        <v>465.4488995503909</v>
+        <v>442.0568695316322</v>
       </c>
       <c r="D155" t="n">
-        <v>44.60048233736705</v>
+        <v>127.3026323701055</v>
       </c>
       <c r="E155" t="n">
-        <v>420.8484172130238</v>
+        <v>314.7542371615267</v>
       </c>
     </row>
     <row r="156">
@@ -3396,16 +3396,16 @@
         </is>
       </c>
       <c r="B156" t="n">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C156" t="n">
-        <v>477.3677024795598</v>
+        <v>453.6932770715935</v>
       </c>
       <c r="D156" t="n">
-        <v>0</v>
+        <v>86.97274601969887</v>
       </c>
       <c r="E156" t="n">
-        <v>477.3677024795598</v>
+        <v>366.7205310518946</v>
       </c>
     </row>
     <row r="157">
@@ -3415,16 +3415,16 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C157" t="n">
-        <v>489.4698320270673</v>
+        <v>465.4488995503909</v>
       </c>
       <c r="D157" t="n">
-        <v>0</v>
+        <v>44.60048233736705</v>
       </c>
       <c r="E157" t="n">
-        <v>489.4698320270673</v>
+        <v>420.8484172130238</v>
       </c>
     </row>
     <row r="158">
@@ -3434,16 +3434,16 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C158" t="n">
-        <v>501.7543083828755</v>
+        <v>477.3677024795598</v>
       </c>
       <c r="D158" t="n">
         <v>0</v>
       </c>
       <c r="E158" t="n">
-        <v>501.7543083828755</v>
+        <v>477.3677024795598</v>
       </c>
     </row>
     <row r="159">
@@ -3453,16 +3453,16 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C159" t="n">
-        <v>514.2016734365858</v>
+        <v>489.4698320270673</v>
       </c>
       <c r="D159" t="n">
         <v>0</v>
       </c>
       <c r="E159" t="n">
-        <v>514.2016734365858</v>
+        <v>489.4698320270673</v>
       </c>
     </row>
     <row r="160">
@@ -3472,16 +3472,16 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C160" t="n">
-        <v>526.7764263467578</v>
+        <v>501.7543083828755</v>
       </c>
       <c r="D160" t="n">
         <v>0</v>
       </c>
       <c r="E160" t="n">
-        <v>526.7764263467578</v>
+        <v>501.7543083828755</v>
       </c>
     </row>
     <row r="161">
@@ -3491,16 +3491,16 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C161" t="n">
-        <v>539.4293574238787</v>
+        <v>514.2016734365858</v>
       </c>
       <c r="D161" t="n">
         <v>0</v>
       </c>
       <c r="E161" t="n">
-        <v>539.4293574238787</v>
+        <v>514.2016734365858</v>
       </c>
     </row>
     <row r="162">
@@ -3510,16 +3510,16 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C162" t="n">
-        <v>552.0995383504245</v>
+        <v>526.7764263467578</v>
       </c>
       <c r="D162" t="n">
         <v>0</v>
       </c>
       <c r="E162" t="n">
-        <v>552.0995383504245</v>
+        <v>526.7764263467578</v>
       </c>
     </row>
     <row r="163">
@@ -3529,16 +3529,16 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C163" t="n">
-        <v>564.7162729342523</v>
+        <v>539.4293574238787</v>
       </c>
       <c r="D163" t="n">
         <v>0</v>
       </c>
       <c r="E163" t="n">
-        <v>564.7162729342523</v>
+        <v>539.4293574238787</v>
       </c>
     </row>
     <row r="164">
@@ -3548,16 +3548,16 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C164" t="n">
-        <v>577.2046819394093</v>
+        <v>552.0995383504245</v>
       </c>
       <c r="D164" t="n">
         <v>0</v>
       </c>
       <c r="E164" t="n">
-        <v>577.2046819394093</v>
+        <v>552.0995383504245</v>
       </c>
     </row>
     <row r="165">
@@ -3567,16 +3567,16 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C165" t="n">
-        <v>589.5024063202416</v>
+        <v>564.7162729342523</v>
       </c>
       <c r="D165" t="n">
         <v>0</v>
       </c>
       <c r="E165" t="n">
-        <v>589.5024063202416</v>
+        <v>564.7162729342523</v>
       </c>
     </row>
     <row r="166">
@@ -3586,16 +3586,16 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C166" t="n">
-        <v>601.5621092435072</v>
+        <v>577.2046819394093</v>
       </c>
       <c r="D166" t="n">
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>601.5621092435072</v>
+        <v>577.2046819394093</v>
       </c>
     </row>
     <row r="167">
@@ -3605,16 +3605,16 @@
         </is>
       </c>
       <c r="B167" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C167" t="n">
-        <v>613.3499229367831</v>
+        <v>589.5024063202416</v>
       </c>
       <c r="D167" t="n">
         <v>0</v>
       </c>
       <c r="E167" t="n">
-        <v>613.3499229367831</v>
+        <v>589.5024063202416</v>
       </c>
     </row>
     <row r="168">
@@ -3624,16 +3624,16 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C168" t="n">
-        <v>624.8439844567928</v>
+        <v>601.5621092435072</v>
       </c>
       <c r="D168" t="n">
         <v>0</v>
       </c>
       <c r="E168" t="n">
-        <v>624.8439844567928</v>
+        <v>601.5621092435072</v>
       </c>
     </row>
     <row r="169">
@@ -3643,16 +3643,16 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C169" t="n">
-        <v>636.033249311631</v>
+        <v>613.3499229367831</v>
       </c>
       <c r="D169" t="n">
         <v>0</v>
       </c>
       <c r="E169" t="n">
-        <v>636.033249311631</v>
+        <v>613.3499229367831</v>
       </c>
     </row>
     <row r="170">
@@ -3662,16 +3662,16 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C170" t="n">
-        <v>646.91637655569</v>
+        <v>624.8439844567928</v>
       </c>
       <c r="D170" t="n">
         <v>0</v>
       </c>
       <c r="E170" t="n">
-        <v>646.91637655569</v>
+        <v>624.8439844567928</v>
       </c>
     </row>
     <row r="171">
@@ -3681,16 +3681,16 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C171" t="n">
-        <v>657.5009633814547</v>
+        <v>636.033249311631</v>
       </c>
       <c r="D171" t="n">
         <v>0</v>
       </c>
       <c r="E171" t="n">
-        <v>657.5009633814547</v>
+        <v>636.033249311631</v>
       </c>
     </row>
     <row r="172">
@@ -3700,16 +3700,16 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C172" t="n">
-        <v>667.8028174620212</v>
+        <v>646.91637655569</v>
       </c>
       <c r="D172" t="n">
         <v>0</v>
       </c>
       <c r="E172" t="n">
-        <v>667.8028174620212</v>
+        <v>646.91637655569</v>
       </c>
     </row>
     <row r="173">
@@ -3719,16 +3719,16 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C173" t="n">
-        <v>677.8457002273666</v>
+        <v>657.5009633814547</v>
       </c>
       <c r="D173" t="n">
         <v>0</v>
       </c>
       <c r="E173" t="n">
-        <v>677.8457002273666</v>
+        <v>657.5009633814547</v>
       </c>
     </row>
     <row r="174">
@@ -3738,16 +3738,16 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C174" t="n">
-        <v>687.6611732954344</v>
+        <v>667.8028174620212</v>
       </c>
       <c r="D174" t="n">
         <v>0</v>
       </c>
       <c r="E174" t="n">
-        <v>687.6611732954344</v>
+        <v>667.8028174620212</v>
       </c>
     </row>
     <row r="175">
@@ -3757,16 +3757,16 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C175" t="n">
-        <v>697.2887683808701</v>
+        <v>677.8457002273666</v>
       </c>
       <c r="D175" t="n">
         <v>0</v>
       </c>
       <c r="E175" t="n">
-        <v>697.2887683808701</v>
+        <v>677.8457002273666</v>
       </c>
     </row>
     <row r="176">
@@ -3776,16 +3776,16 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C176" t="n">
-        <v>706.7763727293656</v>
+        <v>687.6611732954344</v>
       </c>
       <c r="D176" t="n">
         <v>0</v>
       </c>
       <c r="E176" t="n">
-        <v>706.7763727293656</v>
+        <v>687.6611732954344</v>
       </c>
     </row>
     <row r="177">
@@ -3795,16 +3795,16 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C177" t="n">
-        <v>716.1810755069272</v>
+        <v>697.2887683808701</v>
       </c>
       <c r="D177" t="n">
         <v>0</v>
       </c>
       <c r="E177" t="n">
-        <v>716.1810755069272</v>
+        <v>697.2887683808701</v>
       </c>
     </row>
     <row r="178">
@@ -3814,16 +3814,16 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C178" t="n">
-        <v>725.5702078640651</v>
+        <v>706.7763727293656</v>
       </c>
       <c r="D178" t="n">
         <v>0</v>
       </c>
       <c r="E178" t="n">
-        <v>725.5702078640651</v>
+        <v>706.7763727293656</v>
       </c>
     </row>
     <row r="179">
@@ -3833,16 +3833,16 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C179" t="n">
-        <v>735.0124501500986</v>
+        <v>716.1810755069272</v>
       </c>
       <c r="D179" t="n">
         <v>0</v>
       </c>
       <c r="E179" t="n">
-        <v>735.0124501500986</v>
+        <v>716.1810755069272</v>
       </c>
     </row>
     <row r="180">
@@ -3852,16 +3852,16 @@
         </is>
       </c>
       <c r="B180" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C180" t="n">
-        <v>744.5405811415076</v>
+        <v>725.5702078640651</v>
       </c>
       <c r="D180" t="n">
         <v>0</v>
       </c>
       <c r="E180" t="n">
-        <v>744.5405811415076</v>
+        <v>725.5702078640651</v>
       </c>
     </row>
     <row r="181">
@@ -3871,16 +3871,16 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C181" t="n">
-        <v>754.1474722001541</v>
+        <v>735.0124501500986</v>
       </c>
       <c r="D181" t="n">
         <v>0</v>
       </c>
       <c r="E181" t="n">
-        <v>754.1474722001541</v>
+        <v>735.0124501500986</v>
       </c>
     </row>
     <row r="182">
@@ -3890,16 +3890,16 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C182" t="n">
-        <v>763.7915838971441</v>
+        <v>744.5405811415076</v>
       </c>
       <c r="D182" t="n">
         <v>0</v>
       </c>
       <c r="E182" t="n">
-        <v>763.7915838971441</v>
+        <v>744.5405811415076</v>
       </c>
     </row>
     <row r="183">
@@ -3909,16 +3909,16 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C183" t="n">
-        <v>773.4018132692048</v>
+        <v>754.1474722001541</v>
       </c>
       <c r="D183" t="n">
         <v>0</v>
       </c>
       <c r="E183" t="n">
-        <v>773.4018132692048</v>
+        <v>754.1474722001541</v>
       </c>
     </row>
     <row r="184">
@@ -3928,16 +3928,16 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C184" t="n">
-        <v>782.8807984520334</v>
+        <v>763.7915838971441</v>
       </c>
       <c r="D184" t="n">
         <v>0</v>
       </c>
       <c r="E184" t="n">
-        <v>782.8807984520334</v>
+        <v>763.7915838971441</v>
       </c>
     </row>
     <row r="185">
@@ -3947,16 +3947,16 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C185" t="n">
-        <v>792.1064463751992</v>
+        <v>773.4018132692048</v>
       </c>
       <c r="D185" t="n">
         <v>0</v>
       </c>
       <c r="E185" t="n">
-        <v>792.1064463751992</v>
+        <v>773.4018132692048</v>
       </c>
     </row>
     <row r="186">
@@ -3966,16 +3966,16 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C186" t="n">
-        <v>801.0055625499658</v>
+        <v>782.8807984520334</v>
       </c>
       <c r="D186" t="n">
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>801.0055625499658</v>
+        <v>782.8807984520334</v>
       </c>
     </row>
     <row r="187">
@@ -3985,16 +3985,16 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C187" t="n">
-        <v>809.5702750661578</v>
+        <v>792.1064463751992</v>
       </c>
       <c r="D187" t="n">
         <v>0</v>
       </c>
       <c r="E187" t="n">
-        <v>809.5702750661578</v>
+        <v>792.1064463751992</v>
       </c>
     </row>
     <row r="188">
@@ -4004,16 +4004,16 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C188" t="n">
-        <v>817.7966791067724</v>
+        <v>801.0055625499658</v>
       </c>
       <c r="D188" t="n">
         <v>0</v>
       </c>
       <c r="E188" t="n">
-        <v>817.7966791067724</v>
+        <v>801.0055625499658</v>
       </c>
     </row>
     <row r="189">
@@ -4023,16 +4023,16 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C189" t="n">
-        <v>825.6841980525464</v>
+        <v>809.5702750661578</v>
       </c>
       <c r="D189" t="n">
         <v>0</v>
       </c>
       <c r="E189" t="n">
-        <v>825.6841980525464</v>
+        <v>809.5702750661578</v>
       </c>
     </row>
     <row r="190">
@@ -4042,16 +4042,16 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C190" t="n">
-        <v>833.2350515675751</v>
+        <v>817.7966791067724</v>
       </c>
       <c r="D190" t="n">
         <v>0</v>
       </c>
       <c r="E190" t="n">
-        <v>833.2350515675751</v>
+        <v>817.7966791067724</v>
       </c>
     </row>
     <row r="191">
@@ -4061,16 +4061,16 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C191" t="n">
-        <v>840.4538293438424</v>
+        <v>825.6841980525464</v>
       </c>
       <c r="D191" t="n">
         <v>0</v>
       </c>
       <c r="E191" t="n">
-        <v>840.4538293438424</v>
+        <v>825.6841980525464</v>
       </c>
     </row>
     <row r="192">
@@ -4080,16 +4080,16 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C192" t="n">
-        <v>847.3469894257621</v>
+        <v>833.2350515675751</v>
       </c>
       <c r="D192" t="n">
         <v>0</v>
       </c>
       <c r="E192" t="n">
-        <v>847.3469894257621</v>
+        <v>833.2350515675751</v>
       </c>
     </row>
     <row r="193">
@@ -4099,16 +4099,16 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C193" t="n">
-        <v>853.9225262224796</v>
+        <v>840.4538293438424</v>
       </c>
       <c r="D193" t="n">
         <v>0</v>
       </c>
       <c r="E193" t="n">
-        <v>853.9225262224796</v>
+        <v>840.4538293438424</v>
       </c>
     </row>
     <row r="194">
@@ -4118,16 +4118,16 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C194" t="n">
-        <v>860.1896365366114</v>
+        <v>847.3469894257621</v>
       </c>
       <c r="D194" t="n">
         <v>0</v>
       </c>
       <c r="E194" t="n">
-        <v>860.1896365366114</v>
+        <v>847.3469894257621</v>
       </c>
     </row>
     <row r="195">
@@ -4137,16 +4137,16 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C195" t="n">
-        <v>866.1583807445792</v>
+        <v>853.9225262224796</v>
       </c>
       <c r="D195" t="n">
         <v>0</v>
       </c>
       <c r="E195" t="n">
-        <v>866.1583807445792</v>
+        <v>853.9225262224796</v>
       </c>
     </row>
     <row r="196">
@@ -4156,16 +4156,16 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C196" t="n">
-        <v>871.8394764475916</v>
+        <v>860.1896365366114</v>
       </c>
       <c r="D196" t="n">
         <v>0</v>
       </c>
       <c r="E196" t="n">
-        <v>871.8394764475916</v>
+        <v>860.1896365366114</v>
       </c>
     </row>
     <row r="197">
@@ -4175,16 +4175,16 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C197" t="n">
-        <v>877.2440868642597</v>
+        <v>866.1583807445792</v>
       </c>
       <c r="D197" t="n">
         <v>0</v>
       </c>
       <c r="E197" t="n">
-        <v>877.2440868642597</v>
+        <v>866.1583807445792</v>
       </c>
     </row>
     <row r="198">
@@ -4194,16 +4194,16 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C198" t="n">
-        <v>882.3835981021568</v>
+        <v>871.8394764475916</v>
       </c>
       <c r="D198" t="n">
         <v>0</v>
       </c>
       <c r="E198" t="n">
-        <v>882.3835981021568</v>
+        <v>871.8394764475916</v>
       </c>
     </row>
     <row r="199">
@@ -4213,16 +4213,16 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C199" t="n">
-        <v>887.269508719716</v>
+        <v>877.2440868642597</v>
       </c>
       <c r="D199" t="n">
         <v>0</v>
       </c>
       <c r="E199" t="n">
-        <v>887.269508719716</v>
+        <v>877.2440868642597</v>
       </c>
     </row>
     <row r="200">
@@ -4232,16 +4232,16 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C200" t="n">
-        <v>891.9132944745501</v>
+        <v>882.3835981021568</v>
       </c>
       <c r="D200" t="n">
         <v>0</v>
       </c>
       <c r="E200" t="n">
-        <v>891.9132944745501</v>
+        <v>882.3835981021568</v>
       </c>
     </row>
     <row r="201">
@@ -4251,16 +4251,16 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C201" t="n">
-        <v>896.3263095498148</v>
+        <v>887.269508719716</v>
       </c>
       <c r="D201" t="n">
         <v>0</v>
       </c>
       <c r="E201" t="n">
-        <v>896.3263095498148</v>
+        <v>887.269508719716</v>
       </c>
     </row>
     <row r="202">
@@ -4270,16 +4270,16 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C202" t="n">
-        <v>900.5197244440001</v>
+        <v>891.9132944745501</v>
       </c>
       <c r="D202" t="n">
         <v>0</v>
       </c>
       <c r="E202" t="n">
-        <v>900.5197244440001</v>
+        <v>891.9132944745501</v>
       </c>
     </row>
     <row r="203">
@@ -4289,16 +4289,16 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C203" t="n">
-        <v>904.5044346834394</v>
+        <v>896.3263095498148</v>
       </c>
       <c r="D203" t="n">
         <v>0</v>
       </c>
       <c r="E203" t="n">
-        <v>904.5044346834394</v>
+        <v>896.3263095498148</v>
       </c>
     </row>
     <row r="204">
@@ -4308,16 +4308,16 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C204" t="n">
-        <v>908.2910616425326</v>
+        <v>900.5197244440001</v>
       </c>
       <c r="D204" t="n">
         <v>0</v>
       </c>
       <c r="E204" t="n">
-        <v>908.2910616425326</v>
+        <v>900.5197244440001</v>
       </c>
     </row>
     <row r="205">
@@ -4327,16 +4327,16 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C205" t="n">
-        <v>911.889940274173</v>
+        <v>904.5044346834394</v>
       </c>
       <c r="D205" t="n">
         <v>0</v>
       </c>
       <c r="E205" t="n">
-        <v>911.889940274173</v>
+        <v>904.5044346834394</v>
       </c>
     </row>
     <row r="206">
@@ -4346,16 +4346,16 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C206" t="n">
-        <v>915.3111629777907</v>
+        <v>908.2910616425326</v>
       </c>
       <c r="D206" t="n">
         <v>0</v>
       </c>
       <c r="E206" t="n">
-        <v>915.3111629777907</v>
+        <v>908.2910616425326</v>
       </c>
     </row>
     <row r="207">
@@ -4365,16 +4365,16 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C207" t="n">
-        <v>918.5646957836153</v>
+        <v>911.889940274173</v>
       </c>
       <c r="D207" t="n">
         <v>0</v>
       </c>
       <c r="E207" t="n">
-        <v>918.5646957836153</v>
+        <v>911.889940274173</v>
       </c>
     </row>
     <row r="208">
@@ -4384,16 +4384,16 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C208" t="n">
-        <v>921.6607191823343</v>
+        <v>915.3111629777907</v>
       </c>
       <c r="D208" t="n">
         <v>0</v>
       </c>
       <c r="E208" t="n">
-        <v>921.6607191823343</v>
+        <v>915.3111629777907</v>
       </c>
     </row>
     <row r="209">
@@ -4403,16 +4403,16 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C209" t="n">
-        <v>924.6103173140717</v>
+        <v>918.5646957836153</v>
       </c>
       <c r="D209" t="n">
         <v>0</v>
       </c>
       <c r="E209" t="n">
-        <v>924.6103173140717</v>
+        <v>918.5646957836153</v>
       </c>
     </row>
     <row r="210">
@@ -4422,16 +4422,16 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C210" t="n">
-        <v>927.4271759017109</v>
+        <v>921.6607191823343</v>
       </c>
       <c r="D210" t="n">
         <v>0</v>
       </c>
       <c r="E210" t="n">
-        <v>927.4271759017109</v>
+        <v>921.6607191823343</v>
       </c>
     </row>
     <row r="211">
@@ -4441,16 +4441,16 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C211" t="n">
-        <v>930.1317079803973</v>
+        <v>924.6103173140717</v>
       </c>
       <c r="D211" t="n">
         <v>0</v>
       </c>
       <c r="E211" t="n">
-        <v>930.1317079803973</v>
+        <v>924.6103173140717</v>
       </c>
     </row>
     <row r="212">
@@ -4460,16 +4460,16 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C212" t="n">
-        <v>932.7615429562979</v>
+        <v>927.4271759017109</v>
       </c>
       <c r="D212" t="n">
         <v>0</v>
       </c>
       <c r="E212" t="n">
-        <v>932.7615429562979</v>
+        <v>927.4271759017109</v>
       </c>
     </row>
     <row r="213">
@@ -4479,16 +4479,16 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C213" t="n">
-        <v>935.3995452292835</v>
+        <v>930.1317079803973</v>
       </c>
       <c r="D213" t="n">
         <v>0</v>
       </c>
       <c r="E213" t="n">
-        <v>935.3995452292835</v>
+        <v>930.1317079803973</v>
       </c>
     </row>
     <row r="214">
@@ -4498,16 +4498,16 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C214" t="n">
-        <v>938.2521908880295</v>
+        <v>932.7615429562979</v>
       </c>
       <c r="D214" t="n">
         <v>0</v>
       </c>
       <c r="E214" t="n">
-        <v>938.2521908880295</v>
+        <v>932.7615429562979</v>
       </c>
     </row>
     <row r="215">
@@ -4517,16 +4517,16 @@
         </is>
       </c>
       <c r="B215" t="n">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C215" t="n">
-        <v>941.881225254122</v>
+        <v>935.3995452292835</v>
       </c>
       <c r="D215" t="n">
         <v>0</v>
       </c>
       <c r="E215" t="n">
-        <v>941.881225254122</v>
+        <v>935.3995452292835</v>
       </c>
     </row>
     <row r="216">
@@ -4536,16 +4536,16 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C216" t="n">
-        <v>947.9290976331362</v>
+        <v>938.2521908880295</v>
       </c>
       <c r="D216" t="n">
         <v>0</v>
       </c>
       <c r="E216" t="n">
-        <v>947.9290976331362</v>
+        <v>938.2521908880295</v>
       </c>
     </row>
     <row r="217">
@@ -4555,16 +4555,73 @@
         </is>
       </c>
       <c r="B217" t="n">
+        <v>124</v>
+      </c>
+      <c r="C217" t="n">
+        <v>941.881225254122</v>
+      </c>
+      <c r="D217" t="n">
+        <v>0</v>
+      </c>
+      <c r="E217" t="n">
+        <v>941.881225254122</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>GRM95</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>125</v>
+      </c>
+      <c r="C218" t="n">
+        <v>947.9290976331362</v>
+      </c>
+      <c r="D218" t="n">
+        <v>0</v>
+      </c>
+      <c r="E218" t="n">
+        <v>947.9290976331362</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>GRM95</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
         <v>126</v>
       </c>
-      <c r="C217" t="n">
+      <c r="C219" t="n">
         <v>961.5384615384615</v>
       </c>
-      <c r="D217" t="n">
-        <v>0</v>
-      </c>
-      <c r="E217" t="n">
+      <c r="D219" t="n">
+        <v>0</v>
+      </c>
+      <c r="E219" t="n">
         <v>961.5384615384615</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>GRM95</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>127</v>
+      </c>
+      <c r="C220" t="n">
+        <v>961.5384615384614</v>
+      </c>
+      <c r="D220" t="n">
+        <v>0</v>
+      </c>
+      <c r="E220" t="n">
+        <v>961.5384615384614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>